<commit_message>
updated notes and subjects
</commit_message>
<xml_diff>
--- a/subjects.xlsx
+++ b/subjects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="371" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+  <si>
+    <t>Subject Priority</t>
+  </si>
   <si>
     <t>scripting</t>
   </si>
@@ -41,6 +44,9 @@
     <t>Version Control</t>
   </si>
   <si>
+    <t>Algorithms/Data Structures</t>
+  </si>
+  <si>
     <t>Everday scripting with ruby</t>
   </si>
   <si>
@@ -50,9 +56,6 @@
     <t>algorithm design manual</t>
   </si>
   <si>
-    <t>linux </t>
-  </si>
-  <si>
     <t>xUnit test patterns</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
     <t>github</t>
   </si>
   <si>
+    <t>SQL/Xquery</t>
+  </si>
+  <si>
     <t>sql</t>
   </si>
   <si>
@@ -98,13 +104,25 @@
     <t>test driven development</t>
   </si>
   <si>
+    <t>Design Patterns/Clean Code</t>
+  </si>
+  <si>
     <t>apache commons</t>
   </si>
   <si>
     <t>mockito</t>
   </si>
   <si>
+    <t>Functional Programming</t>
+  </si>
+  <si>
     <t>jackson</t>
+  </si>
+  <si>
+    <t>Scripting</t>
+  </si>
+  <si>
+    <t>More Command Line Operations</t>
   </si>
 </sst>
 </file>
@@ -280,21 +298,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6651162790698"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3302325581395"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6651162790698"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6651162790698"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,25 +341,28 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>13</v>
@@ -348,10 +370,13 @@
       <c r="H2" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>15</v>
+      <c r="A3" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
@@ -359,7 +384,7 @@
       <c r="D3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -368,40 +393,65 @@
       <c r="H3" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>21</v>
+      <c r="A4" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>24</v>
+      <c r="A5" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>28</v>
+      <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>29</v>
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>